<commit_message>
added sensor data from Joung et al 2017 supplementary materials
</commit_message>
<xml_diff>
--- a/01_raw data/Joung et al. Supp Data.xlsx
+++ b/01_raw data/Joung et al. Supp Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinkincaid/ownCloud/bree_frozeN/01_raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2D574-0A8E-FB44-82B5-844E24674F9F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337AFCBC-B5BA-8846-9E4B-B42E748F7896}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1260" windowWidth="32080" windowHeight="21180" activeTab="1" xr2:uid="{07636632-EDCE-D346-9015-615D5D59BF0A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{07636632-EDCE-D346-9015-615D5D59BF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Miss Bay 2015 Data - Supp Info" sheetId="1" r:id="rId1"/>
@@ -357,15 +357,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,6 +367,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,7 +697,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="10.83203125" style="28"/>
-    <col min="5" max="5" width="10.83203125" style="38"/>
+    <col min="5" max="5" width="10.83203125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="32" t="s">
         <v>41</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -782,10 +782,10 @@
       <c r="AA1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AB1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="33"/>
+      <c r="AC1" s="37"/>
       <c r="AD1" s="2" t="s">
         <v>37</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="33" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -854,7 +854,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B3" s="26">
         <v>15</v>
@@ -865,7 +865,7 @@
       <c r="D3" s="7">
         <v>0.34</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="34">
         <v>0.4</v>
       </c>
       <c r="F3" s="8">
@@ -919,8 +919,8 @@
       <c r="Z3" s="10">
         <v>0.26</v>
       </c>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
       <c r="AC3" s="8"/>
       <c r="AD3" s="7">
         <v>0.32</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B4" s="26">
         <v>15</v>
@@ -942,7 +942,7 @@
       <c r="D4" s="7">
         <v>0.34</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="34">
         <v>0.9</v>
       </c>
       <c r="F4" s="8">
@@ -980,15 +980,15 @@
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="12"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="11"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B5" s="26">
         <v>15</v>
@@ -999,7 +999,7 @@
       <c r="D5" s="7">
         <v>0.34</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="34">
         <v>1.4</v>
       </c>
       <c r="F5" s="8">
@@ -1037,15 +1037,15 @@
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="12"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36"/>
       <c r="AC5" s="8"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="11"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B6" s="26">
         <v>15</v>
@@ -1056,7 +1056,7 @@
       <c r="D6" s="7">
         <v>0.34</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="34">
         <v>1.9</v>
       </c>
       <c r="F6" s="8">
@@ -1094,15 +1094,15 @@
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="12"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="11"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B7" s="26">
         <v>15</v>
@@ -1113,7 +1113,7 @@
       <c r="D7" s="7">
         <v>0.34</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="34">
         <v>2.4</v>
       </c>
       <c r="F7" s="8">
@@ -1167,10 +1167,10 @@
       <c r="Z7" s="10">
         <v>0.64</v>
       </c>
-      <c r="AA7" s="32">
+      <c r="AA7" s="36">
         <v>0.13</v>
       </c>
-      <c r="AB7" s="32"/>
+      <c r="AB7" s="36"/>
       <c r="AC7" s="8">
         <v>0.2</v>
       </c>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B8" s="26">
         <v>15</v>
@@ -1194,7 +1194,7 @@
       <c r="D8" s="7">
         <v>0.34</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="34">
         <v>2.6</v>
       </c>
       <c r="F8" s="8">
@@ -1232,15 +1232,15 @@
       <c r="X8" s="9"/>
       <c r="Y8" s="9"/>
       <c r="Z8" s="12"/>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="32"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="11"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B9" s="26">
         <v>15</v>
@@ -1251,7 +1251,7 @@
       <c r="D9" s="7">
         <v>0.34</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="34">
         <v>2.9</v>
       </c>
       <c r="F9" s="8">
@@ -1305,10 +1305,10 @@
       <c r="Z9" s="10">
         <v>1.94</v>
       </c>
-      <c r="AA9" s="32">
+      <c r="AA9" s="36">
         <v>0.15</v>
       </c>
-      <c r="AB9" s="32"/>
+      <c r="AB9" s="36"/>
       <c r="AC9" s="8">
         <v>0.11</v>
       </c>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B10" s="26">
         <v>15</v>
@@ -1332,7 +1332,7 @@
       <c r="D10" s="7">
         <v>0.34</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="34">
         <v>3.1</v>
       </c>
       <c r="F10" s="8">
@@ -1386,10 +1386,10 @@
       <c r="Z10" s="10">
         <v>2.79</v>
       </c>
-      <c r="AA10" s="32">
+      <c r="AA10" s="36">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AB10" s="32"/>
+      <c r="AB10" s="36"/>
       <c r="AC10" s="8">
         <v>0.12</v>
       </c>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B11" s="26">
         <v>15</v>
@@ -1413,7 +1413,7 @@
       <c r="D11" s="7">
         <v>0.34</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="34">
         <v>3.4</v>
       </c>
       <c r="F11" s="8">
@@ -1461,10 +1461,10 @@
       <c r="Z11" s="10">
         <v>5.34</v>
       </c>
-      <c r="AA11" s="32">
+      <c r="AA11" s="36">
         <v>0.12</v>
       </c>
-      <c r="AB11" s="32"/>
+      <c r="AB11" s="36"/>
       <c r="AC11" s="8">
         <v>0.13</v>
       </c>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B12" s="26">
         <v>35</v>
@@ -1488,7 +1488,7 @@
       <c r="D12" s="7">
         <v>0.54</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="34">
         <v>0.9</v>
       </c>
       <c r="F12" s="8">
@@ -1554,10 +1554,10 @@
       <c r="Z12" s="10">
         <v>0.26</v>
       </c>
-      <c r="AA12" s="32">
+      <c r="AA12" s="36">
         <v>0.03</v>
       </c>
-      <c r="AB12" s="32"/>
+      <c r="AB12" s="36"/>
       <c r="AC12" s="8">
         <v>0.14000000000000001</v>
       </c>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B13" s="26">
         <v>35</v>
@@ -1581,7 +1581,7 @@
       <c r="D13" s="7">
         <v>0.54</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13" s="34">
         <v>1.5</v>
       </c>
       <c r="F13" s="8">
@@ -1619,15 +1619,15 @@
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
       <c r="Z13" s="12"/>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32"/>
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="36"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="7"/>
       <c r="AE13" s="11"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B14" s="26">
         <v>35</v>
@@ -1638,7 +1638,7 @@
       <c r="D14" s="7">
         <v>0.54</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="34">
         <v>1.8</v>
       </c>
       <c r="F14" s="8">
@@ -1676,15 +1676,15 @@
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
       <c r="Z14" s="12"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="32"/>
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="36"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="7"/>
       <c r="AE14" s="11"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B15" s="26">
         <v>35</v>
@@ -1695,7 +1695,7 @@
       <c r="D15" s="7">
         <v>0.54</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="34">
         <v>2.1</v>
       </c>
       <c r="F15" s="8">
@@ -1733,15 +1733,15 @@
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="12"/>
-      <c r="AA15" s="32"/>
-      <c r="AB15" s="32"/>
+      <c r="AA15" s="36"/>
+      <c r="AB15" s="36"/>
       <c r="AC15" s="8"/>
       <c r="AD15" s="7"/>
       <c r="AE15" s="11"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B16" s="26">
         <v>35</v>
@@ -1752,7 +1752,7 @@
       <c r="D16" s="7">
         <v>0.54</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="34">
         <v>2.8</v>
       </c>
       <c r="F16" s="8">
@@ -1816,8 +1816,8 @@
         <v>3.24</v>
       </c>
       <c r="Z16" s="12"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="32"/>
+      <c r="AA16" s="36"/>
+      <c r="AB16" s="36"/>
       <c r="AC16" s="8"/>
       <c r="AD16" s="7">
         <v>0.17</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B17" s="26">
         <v>35</v>
@@ -1839,7 +1839,7 @@
       <c r="D17" s="7">
         <v>0.54</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="34">
         <v>3</v>
       </c>
       <c r="F17" s="8">
@@ -1905,10 +1905,10 @@
       <c r="Z17" s="10">
         <v>1.55</v>
       </c>
-      <c r="AA17" s="32">
+      <c r="AA17" s="36">
         <v>0.11</v>
       </c>
-      <c r="AB17" s="32"/>
+      <c r="AB17" s="36"/>
       <c r="AC17" s="8">
         <v>0.09</v>
       </c>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B18" s="26">
         <v>35</v>
@@ -1932,7 +1932,7 @@
       <c r="D18" s="7">
         <v>0.54</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="34">
         <v>3.2</v>
       </c>
       <c r="F18" s="8">
@@ -1996,8 +1996,8 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="Z18" s="12"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="32"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="36"/>
       <c r="AC18" s="8"/>
       <c r="AD18" s="7">
         <v>0.36</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
-        <v>43135</v>
+        <v>42039</v>
       </c>
       <c r="B19" s="26">
         <v>35</v>
@@ -2019,7 +2019,7 @@
       <c r="D19" s="7">
         <v>0.54</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="34">
         <v>3.5</v>
       </c>
       <c r="F19" s="8">
@@ -2085,10 +2085,10 @@
       <c r="Z19" s="10">
         <v>9.3699999999999992</v>
       </c>
-      <c r="AA19" s="32">
+      <c r="AA19" s="36">
         <v>0.11</v>
       </c>
-      <c r="AB19" s="32"/>
+      <c r="AB19" s="36"/>
       <c r="AC19" s="8">
         <v>0.1</v>
       </c>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B20" s="26">
         <v>48</v>
@@ -2112,7 +2112,7 @@
       <c r="D20" s="7">
         <v>0.7</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="34">
         <v>0.7</v>
       </c>
       <c r="F20" s="8">
@@ -2176,10 +2176,10 @@
       <c r="Z20" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AA20" s="32">
+      <c r="AA20" s="36">
         <v>0.06</v>
       </c>
-      <c r="AB20" s="32"/>
+      <c r="AB20" s="36"/>
       <c r="AC20" s="8">
         <v>1.8</v>
       </c>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B21" s="26">
         <v>48</v>
@@ -2203,7 +2203,7 @@
       <c r="D21" s="7">
         <v>0.7</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="34">
         <v>1.2</v>
       </c>
       <c r="F21" s="8">
@@ -2241,15 +2241,15 @@
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="12"/>
-      <c r="AA21" s="32"/>
-      <c r="AB21" s="32"/>
+      <c r="AA21" s="36"/>
+      <c r="AB21" s="36"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="7"/>
       <c r="AE21" s="11"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B22" s="26">
         <v>48</v>
@@ -2260,7 +2260,7 @@
       <c r="D22" s="7">
         <v>0.7</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="34">
         <v>1.8</v>
       </c>
       <c r="F22" s="8">
@@ -2298,15 +2298,15 @@
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="12"/>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="32"/>
+      <c r="AA22" s="36"/>
+      <c r="AB22" s="36"/>
       <c r="AC22" s="8"/>
       <c r="AD22" s="7"/>
       <c r="AE22" s="11"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B23" s="26">
         <v>48</v>
@@ -2317,7 +2317,7 @@
       <c r="D23" s="7">
         <v>0.7</v>
       </c>
-      <c r="E23" s="37">
+      <c r="E23" s="34">
         <v>2.2999999999999998</v>
       </c>
       <c r="F23" s="8">
@@ -2381,8 +2381,8 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="Z23" s="12"/>
-      <c r="AA23" s="32"/>
-      <c r="AB23" s="32"/>
+      <c r="AA23" s="36"/>
+      <c r="AB23" s="36"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="7">
         <v>2.09</v>
@@ -2393,7 +2393,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B24" s="26">
         <v>48</v>
@@ -2404,7 +2404,7 @@
       <c r="D24" s="7">
         <v>0.7</v>
       </c>
-      <c r="E24" s="37">
+      <c r="E24" s="34">
         <v>2.4</v>
       </c>
       <c r="F24" s="8">
@@ -2468,8 +2468,8 @@
         <v>3.49</v>
       </c>
       <c r="Z24" s="12"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="32"/>
+      <c r="AA24" s="36"/>
+      <c r="AB24" s="36"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="7">
         <v>1.5</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B25" s="26">
         <v>48</v>
@@ -2491,7 +2491,7 @@
       <c r="D25" s="7">
         <v>0.7</v>
       </c>
-      <c r="E25" s="37">
+      <c r="E25" s="34">
         <v>2.8</v>
       </c>
       <c r="F25" s="8">
@@ -2557,10 +2557,10 @@
       <c r="Z25" s="10">
         <v>15.73</v>
       </c>
-      <c r="AA25" s="32">
+      <c r="AA25" s="36">
         <v>0.11</v>
       </c>
-      <c r="AB25" s="32"/>
+      <c r="AB25" s="36"/>
       <c r="AC25" s="8">
         <v>2.0499999999999998</v>
       </c>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
-        <v>43148</v>
+        <v>42052</v>
       </c>
       <c r="B26" s="26">
         <v>48</v>
@@ -2584,7 +2584,7 @@
       <c r="D26" s="7">
         <v>0.7</v>
       </c>
-      <c r="E26" s="37">
+      <c r="E26" s="34">
         <v>3.1</v>
       </c>
       <c r="F26" s="8">
@@ -2650,10 +2650,10 @@
       <c r="Z26" s="10">
         <v>23.81</v>
       </c>
-      <c r="AA26" s="32">
+      <c r="AA26" s="36">
         <v>0.09</v>
       </c>
-      <c r="AB26" s="32"/>
+      <c r="AB26" s="36"/>
       <c r="AC26" s="8">
         <v>3.27</v>
       </c>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B27" s="26">
         <v>69</v>
@@ -2677,7 +2677,7 @@
       <c r="D27" s="7">
         <v>0.65</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="34">
         <v>0.7</v>
       </c>
       <c r="F27" s="8">
@@ -2743,10 +2743,10 @@
       <c r="Z27" s="10">
         <v>0.61</v>
       </c>
-      <c r="AA27" s="32">
+      <c r="AA27" s="36">
         <v>0.06</v>
       </c>
-      <c r="AB27" s="32"/>
+      <c r="AB27" s="36"/>
       <c r="AC27" s="8">
         <v>1.92</v>
       </c>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B28" s="26">
         <v>69</v>
@@ -2770,7 +2770,7 @@
       <c r="D28" s="7">
         <v>0.65</v>
       </c>
-      <c r="E28" s="37">
+      <c r="E28" s="34">
         <v>1</v>
       </c>
       <c r="F28" s="8">
@@ -2808,15 +2808,15 @@
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
       <c r="Z28" s="12"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="32"/>
+      <c r="AA28" s="36"/>
+      <c r="AB28" s="36"/>
       <c r="AC28" s="8"/>
       <c r="AD28" s="7"/>
       <c r="AE28" s="11"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B29" s="26">
         <v>69</v>
@@ -2827,7 +2827,7 @@
       <c r="D29" s="7">
         <v>0.65</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E29" s="34">
         <v>1.3</v>
       </c>
       <c r="F29" s="8">
@@ -2861,15 +2861,15 @@
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="12"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
+      <c r="AA29" s="36"/>
+      <c r="AB29" s="36"/>
       <c r="AC29" s="8"/>
       <c r="AD29" s="7"/>
       <c r="AE29" s="11"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B30" s="26">
         <v>69</v>
@@ -2880,7 +2880,7 @@
       <c r="D30" s="7">
         <v>0.65</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E30" s="34">
         <v>1.6</v>
       </c>
       <c r="F30" s="8">
@@ -2918,15 +2918,15 @@
       <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
       <c r="Z30" s="12"/>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="32"/>
+      <c r="AA30" s="36"/>
+      <c r="AB30" s="36"/>
       <c r="AC30" s="8"/>
       <c r="AD30" s="7"/>
       <c r="AE30" s="11"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B31" s="26">
         <v>69</v>
@@ -2937,7 +2937,7 @@
       <c r="D31" s="7">
         <v>0.65</v>
       </c>
-      <c r="E31" s="37">
+      <c r="E31" s="34">
         <v>1.9</v>
       </c>
       <c r="F31" s="8">
@@ -3001,8 +3001,8 @@
         <v>2.63</v>
       </c>
       <c r="Z31" s="12"/>
-      <c r="AA31" s="32"/>
-      <c r="AB31" s="32"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
       <c r="AC31" s="8"/>
       <c r="AD31" s="7">
         <v>3.11</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B32" s="26">
         <v>69</v>
@@ -3024,7 +3024,7 @@
       <c r="D32" s="7">
         <v>0.65</v>
       </c>
-      <c r="E32" s="37">
+      <c r="E32" s="34">
         <v>2.1</v>
       </c>
       <c r="F32" s="8">
@@ -3058,15 +3058,15 @@
       <c r="X32" s="9"/>
       <c r="Y32" s="9"/>
       <c r="Z32" s="12"/>
-      <c r="AA32" s="32"/>
-      <c r="AB32" s="32"/>
+      <c r="AA32" s="36"/>
+      <c r="AB32" s="36"/>
       <c r="AC32" s="8"/>
       <c r="AD32" s="7"/>
       <c r="AE32" s="11"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B33" s="26">
         <v>69</v>
@@ -3077,7 +3077,7 @@
       <c r="D33" s="7">
         <v>0.65</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="34">
         <v>2.4</v>
       </c>
       <c r="F33" s="8">
@@ -3141,8 +3141,8 @@
         <v>2.23</v>
       </c>
       <c r="Z33" s="12"/>
-      <c r="AA33" s="32"/>
-      <c r="AB33" s="32"/>
+      <c r="AA33" s="36"/>
+      <c r="AB33" s="36"/>
       <c r="AC33" s="8"/>
       <c r="AD33" s="7">
         <v>2.2000000000000002</v>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B34" s="26">
         <v>69</v>
@@ -3164,7 +3164,7 @@
       <c r="D34" s="7">
         <v>0.65</v>
       </c>
-      <c r="E34" s="37">
+      <c r="E34" s="34">
         <v>2.7</v>
       </c>
       <c r="F34" s="8">
@@ -3230,10 +3230,10 @@
       <c r="Z34" s="10">
         <v>24.76</v>
       </c>
-      <c r="AA34" s="32">
+      <c r="AA34" s="36">
         <v>0.08</v>
       </c>
-      <c r="AB34" s="32"/>
+      <c r="AB34" s="36"/>
       <c r="AC34" s="8">
         <v>3.26</v>
       </c>
@@ -3246,7 +3246,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B35" s="26">
         <v>69</v>
@@ -3257,7 +3257,7 @@
       <c r="D35" s="7">
         <v>0.65</v>
       </c>
-      <c r="E35" s="37">
+      <c r="E35" s="34">
         <v>2.9</v>
       </c>
       <c r="F35" s="8">
@@ -3323,10 +3323,10 @@
       <c r="Z35" s="10">
         <v>38.57</v>
       </c>
-      <c r="AA35" s="32">
+      <c r="AA35" s="36">
         <v>0.1</v>
       </c>
-      <c r="AB35" s="32"/>
+      <c r="AB35" s="36"/>
       <c r="AC35" s="8">
         <v>3.88</v>
       </c>
@@ -3339,7 +3339,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B36" s="26">
         <v>78</v>
@@ -3350,7 +3350,7 @@
       <c r="D36" s="7">
         <v>0.67</v>
       </c>
-      <c r="E36" s="37">
+      <c r="E36" s="34">
         <v>0.6</v>
       </c>
       <c r="F36" s="8">
@@ -3416,10 +3416,10 @@
       <c r="Z36" s="10">
         <v>0.88</v>
       </c>
-      <c r="AA36" s="32">
+      <c r="AA36" s="36">
         <v>0.42</v>
       </c>
-      <c r="AB36" s="32"/>
+      <c r="AB36" s="36"/>
       <c r="AC36" s="8">
         <v>1.97</v>
       </c>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B37" s="26">
         <v>78</v>
@@ -3443,7 +3443,7 @@
       <c r="D37" s="7">
         <v>0.67</v>
       </c>
-      <c r="E37" s="37">
+      <c r="E37" s="34">
         <v>1</v>
       </c>
       <c r="F37" s="8">
@@ -3479,15 +3479,15 @@
       <c r="X37" s="9"/>
       <c r="Y37" s="9"/>
       <c r="Z37" s="12"/>
-      <c r="AA37" s="32"/>
-      <c r="AB37" s="32"/>
+      <c r="AA37" s="36"/>
+      <c r="AB37" s="36"/>
       <c r="AC37" s="8"/>
       <c r="AD37" s="7"/>
       <c r="AE37" s="11"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B38" s="26">
         <v>78</v>
@@ -3498,7 +3498,7 @@
       <c r="D38" s="7">
         <v>0.67</v>
       </c>
-      <c r="E38" s="37">
+      <c r="E38" s="34">
         <v>1.3</v>
       </c>
       <c r="F38" s="8">
@@ -3532,15 +3532,15 @@
       <c r="X38" s="9"/>
       <c r="Y38" s="9"/>
       <c r="Z38" s="12"/>
-      <c r="AA38" s="32"/>
-      <c r="AB38" s="32"/>
+      <c r="AA38" s="36"/>
+      <c r="AB38" s="36"/>
       <c r="AC38" s="8"/>
       <c r="AD38" s="7"/>
       <c r="AE38" s="11"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B39" s="26">
         <v>78</v>
@@ -3551,7 +3551,7 @@
       <c r="D39" s="7">
         <v>0.67</v>
       </c>
-      <c r="E39" s="37">
+      <c r="E39" s="34">
         <v>1.5</v>
       </c>
       <c r="F39" s="8">
@@ -3587,15 +3587,15 @@
       <c r="X39" s="9"/>
       <c r="Y39" s="9"/>
       <c r="Z39" s="12"/>
-      <c r="AA39" s="32"/>
-      <c r="AB39" s="32"/>
+      <c r="AA39" s="36"/>
+      <c r="AB39" s="36"/>
       <c r="AC39" s="8"/>
       <c r="AD39" s="7"/>
       <c r="AE39" s="11"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B40" s="26">
         <v>78</v>
@@ -3606,7 +3606,7 @@
       <c r="D40" s="7">
         <v>0.67</v>
       </c>
-      <c r="E40" s="37">
+      <c r="E40" s="34">
         <v>1.8</v>
       </c>
       <c r="F40" s="8">
@@ -3642,15 +3642,15 @@
       <c r="X40" s="9"/>
       <c r="Y40" s="9"/>
       <c r="Z40" s="12"/>
-      <c r="AA40" s="32"/>
-      <c r="AB40" s="32"/>
+      <c r="AA40" s="36"/>
+      <c r="AB40" s="36"/>
       <c r="AC40" s="8"/>
       <c r="AD40" s="7"/>
       <c r="AE40" s="11"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B41" s="26">
         <v>78</v>
@@ -3661,7 +3661,7 @@
       <c r="D41" s="7">
         <v>0.67</v>
       </c>
-      <c r="E41" s="37">
+      <c r="E41" s="34">
         <v>2.2000000000000002</v>
       </c>
       <c r="F41" s="8">
@@ -3723,8 +3723,8 @@
         <v>2.74</v>
       </c>
       <c r="Z41" s="12"/>
-      <c r="AA41" s="32"/>
-      <c r="AB41" s="32"/>
+      <c r="AA41" s="36"/>
+      <c r="AB41" s="36"/>
       <c r="AC41" s="8"/>
       <c r="AD41" s="7">
         <v>2.2200000000000002</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B42" s="26">
         <v>78</v>
@@ -3746,7 +3746,7 @@
       <c r="D42" s="7">
         <v>0.67</v>
       </c>
-      <c r="E42" s="37">
+      <c r="E42" s="34">
         <v>2.6</v>
       </c>
       <c r="F42" s="8">
@@ -3808,8 +3808,8 @@
         <v>2.19</v>
       </c>
       <c r="Z42" s="12"/>
-      <c r="AA42" s="32"/>
-      <c r="AB42" s="32"/>
+      <c r="AA42" s="36"/>
+      <c r="AB42" s="36"/>
       <c r="AC42" s="8"/>
       <c r="AD42" s="7">
         <v>3.14</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B43" s="26">
         <v>78</v>
@@ -3831,7 +3831,7 @@
       <c r="D43" s="7">
         <v>0.67</v>
       </c>
-      <c r="E43" s="37">
+      <c r="E43" s="34">
         <v>2.9</v>
       </c>
       <c r="F43" s="8">
@@ -3897,10 +3897,10 @@
       <c r="Z43" s="10">
         <v>24.09</v>
       </c>
-      <c r="AA43" s="32">
+      <c r="AA43" s="36">
         <v>0.08</v>
       </c>
-      <c r="AB43" s="32"/>
+      <c r="AB43" s="36"/>
       <c r="AC43" s="8">
         <v>3.13</v>
       </c>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B44" s="26">
         <v>78</v>
@@ -3924,7 +3924,7 @@
       <c r="D44" s="7">
         <v>0.67</v>
       </c>
-      <c r="E44" s="37">
+      <c r="E44" s="34">
         <v>3</v>
       </c>
       <c r="F44" s="8">
@@ -3986,10 +3986,10 @@
       <c r="Z44" s="10">
         <v>26.28</v>
       </c>
-      <c r="AA44" s="32">
+      <c r="AA44" s="36">
         <v>0.06</v>
       </c>
-      <c r="AB44" s="32"/>
+      <c r="AB44" s="36"/>
       <c r="AC44" s="8">
         <v>3.45</v>
       </c>
@@ -4002,7 +4002,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B45" s="26">
         <v>84</v>
@@ -4013,7 +4013,7 @@
       <c r="D45" s="7">
         <v>0.7</v>
       </c>
-      <c r="E45" s="37">
+      <c r="E45" s="34">
         <v>0.7</v>
       </c>
       <c r="F45" s="8">
@@ -4079,10 +4079,10 @@
       <c r="Z45" s="10">
         <v>0.8</v>
       </c>
-      <c r="AA45" s="32">
+      <c r="AA45" s="36">
         <v>0.13</v>
       </c>
-      <c r="AB45" s="32"/>
+      <c r="AB45" s="36"/>
       <c r="AC45" s="8">
         <v>2.86</v>
       </c>
@@ -4095,7 +4095,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B46" s="26">
         <v>84</v>
@@ -4106,7 +4106,7 @@
       <c r="D46" s="7">
         <v>0.7</v>
       </c>
-      <c r="E46" s="37">
+      <c r="E46" s="34">
         <v>0.9</v>
       </c>
       <c r="F46" s="8">
@@ -4144,15 +4144,15 @@
       <c r="X46" s="9"/>
       <c r="Y46" s="9"/>
       <c r="Z46" s="12"/>
-      <c r="AA46" s="32"/>
-      <c r="AB46" s="32"/>
+      <c r="AA46" s="36"/>
+      <c r="AB46" s="36"/>
       <c r="AC46" s="8"/>
       <c r="AD46" s="7"/>
       <c r="AE46" s="11"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B47" s="26">
         <v>84</v>
@@ -4163,7 +4163,7 @@
       <c r="D47" s="7">
         <v>0.7</v>
       </c>
-      <c r="E47" s="37">
+      <c r="E47" s="34">
         <v>1.3</v>
       </c>
       <c r="F47" s="8">
@@ -4197,15 +4197,15 @@
       <c r="X47" s="9"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="12"/>
-      <c r="AA47" s="32"/>
-      <c r="AB47" s="32"/>
+      <c r="AA47" s="36"/>
+      <c r="AB47" s="36"/>
       <c r="AC47" s="8"/>
       <c r="AD47" s="7"/>
       <c r="AE47" s="11"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B48" s="26">
         <v>84</v>
@@ -4216,7 +4216,7 @@
       <c r="D48" s="7">
         <v>0.7</v>
       </c>
-      <c r="E48" s="37">
+      <c r="E48" s="34">
         <v>1.6</v>
       </c>
       <c r="F48" s="8">
@@ -4252,15 +4252,15 @@
       <c r="X48" s="9"/>
       <c r="Y48" s="9"/>
       <c r="Z48" s="12"/>
-      <c r="AA48" s="32"/>
-      <c r="AB48" s="32"/>
+      <c r="AA48" s="36"/>
+      <c r="AB48" s="36"/>
       <c r="AC48" s="8"/>
       <c r="AD48" s="7"/>
       <c r="AE48" s="11"/>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B49" s="26">
         <v>84</v>
@@ -4271,7 +4271,7 @@
       <c r="D49" s="7">
         <v>0.7</v>
       </c>
-      <c r="E49" s="37">
+      <c r="E49" s="34">
         <v>1.8</v>
       </c>
       <c r="F49" s="8">
@@ -4305,15 +4305,15 @@
       <c r="X49" s="9"/>
       <c r="Y49" s="9"/>
       <c r="Z49" s="12"/>
-      <c r="AA49" s="32"/>
-      <c r="AB49" s="32"/>
+      <c r="AA49" s="36"/>
+      <c r="AB49" s="36"/>
       <c r="AC49" s="8"/>
       <c r="AD49" s="7"/>
       <c r="AE49" s="11"/>
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B50" s="26">
         <v>84</v>
@@ -4324,7 +4324,7 @@
       <c r="D50" s="7">
         <v>0.7</v>
       </c>
-      <c r="E50" s="37">
+      <c r="E50" s="34">
         <v>2.1</v>
       </c>
       <c r="F50" s="8">
@@ -4386,8 +4386,8 @@
         <v>2.76</v>
       </c>
       <c r="Z50" s="12"/>
-      <c r="AA50" s="32"/>
-      <c r="AB50" s="32"/>
+      <c r="AA50" s="36"/>
+      <c r="AB50" s="36"/>
       <c r="AC50" s="8"/>
       <c r="AD50" s="7">
         <v>2.5</v>
@@ -4398,7 +4398,7 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B51" s="26">
         <v>84</v>
@@ -4409,7 +4409,7 @@
       <c r="D51" s="7">
         <v>0.7</v>
       </c>
-      <c r="E51" s="37">
+      <c r="E51" s="34">
         <v>2.4</v>
       </c>
       <c r="F51" s="8">
@@ -4473,8 +4473,8 @@
         <v>2.31</v>
       </c>
       <c r="Z51" s="12"/>
-      <c r="AA51" s="32"/>
-      <c r="AB51" s="32"/>
+      <c r="AA51" s="36"/>
+      <c r="AB51" s="36"/>
       <c r="AC51" s="8"/>
       <c r="AD51" s="7">
         <v>2.9</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B52" s="26">
         <v>84</v>
@@ -4496,7 +4496,7 @@
       <c r="D52" s="7">
         <v>0.7</v>
       </c>
-      <c r="E52" s="37">
+      <c r="E52" s="34">
         <v>2.5</v>
       </c>
       <c r="F52" s="8">
@@ -4532,15 +4532,15 @@
       <c r="X52" s="9"/>
       <c r="Y52" s="9"/>
       <c r="Z52" s="12"/>
-      <c r="AA52" s="32"/>
-      <c r="AB52" s="32"/>
+      <c r="AA52" s="36"/>
+      <c r="AB52" s="36"/>
       <c r="AC52" s="8"/>
       <c r="AD52" s="7"/>
       <c r="AE52" s="11"/>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A53" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B53" s="26">
         <v>84</v>
@@ -4551,7 +4551,7 @@
       <c r="D53" s="7">
         <v>0.7</v>
       </c>
-      <c r="E53" s="37">
+      <c r="E53" s="34">
         <v>2.8</v>
       </c>
       <c r="F53" s="8">
@@ -4615,10 +4615,10 @@
       <c r="Z53" s="10">
         <v>18.98</v>
       </c>
-      <c r="AA53" s="32">
+      <c r="AA53" s="36">
         <v>0.11</v>
       </c>
-      <c r="AB53" s="32"/>
+      <c r="AB53" s="36"/>
       <c r="AC53" s="8">
         <v>2.81</v>
       </c>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A54" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B54" s="26">
         <v>84</v>
@@ -4642,7 +4642,7 @@
       <c r="D54" s="7">
         <v>0.7</v>
       </c>
-      <c r="E54" s="37">
+      <c r="E54" s="34">
         <v>3</v>
       </c>
       <c r="F54" s="8">
@@ -4704,10 +4704,10 @@
       <c r="Z54" s="10">
         <v>24.17</v>
       </c>
-      <c r="AA54" s="32">
+      <c r="AA54" s="36">
         <v>0.06</v>
       </c>
-      <c r="AB54" s="32"/>
+      <c r="AB54" s="36"/>
       <c r="AC54" s="8">
         <v>3.43</v>
       </c>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A55" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B55" s="26">
         <v>87</v>
@@ -4731,7 +4731,7 @@
       <c r="D55" s="7">
         <v>0.69</v>
       </c>
-      <c r="E55" s="37">
+      <c r="E55" s="34">
         <v>0.7</v>
       </c>
       <c r="F55" s="8">
@@ -4797,10 +4797,10 @@
       <c r="Z55" s="10">
         <v>0.91</v>
       </c>
-      <c r="AA55" s="32">
+      <c r="AA55" s="36">
         <v>0.11</v>
       </c>
-      <c r="AB55" s="32"/>
+      <c r="AB55" s="36"/>
       <c r="AC55" s="8">
         <v>2.87</v>
       </c>
@@ -4813,7 +4813,7 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A56" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B56" s="26">
         <v>87</v>
@@ -4824,7 +4824,7 @@
       <c r="D56" s="7">
         <v>0.69</v>
       </c>
-      <c r="E56" s="37">
+      <c r="E56" s="34">
         <v>1</v>
       </c>
       <c r="F56" s="8">
@@ -4862,15 +4862,15 @@
       <c r="X56" s="9"/>
       <c r="Y56" s="9"/>
       <c r="Z56" s="12"/>
-      <c r="AA56" s="32"/>
-      <c r="AB56" s="32"/>
+      <c r="AA56" s="36"/>
+      <c r="AB56" s="36"/>
       <c r="AC56" s="8"/>
       <c r="AD56" s="7"/>
       <c r="AE56" s="11"/>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A57" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B57" s="26">
         <v>87</v>
@@ -4881,7 +4881,7 @@
       <c r="D57" s="7">
         <v>0.69</v>
       </c>
-      <c r="E57" s="37">
+      <c r="E57" s="34">
         <v>1.2</v>
       </c>
       <c r="F57" s="8">
@@ -4915,15 +4915,15 @@
       <c r="X57" s="9"/>
       <c r="Y57" s="9"/>
       <c r="Z57" s="12"/>
-      <c r="AA57" s="32"/>
-      <c r="AB57" s="32"/>
+      <c r="AA57" s="36"/>
+      <c r="AB57" s="36"/>
       <c r="AC57" s="8"/>
       <c r="AD57" s="7"/>
       <c r="AE57" s="11"/>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A58" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B58" s="26">
         <v>87</v>
@@ -4934,7 +4934,7 @@
       <c r="D58" s="7">
         <v>0.69</v>
       </c>
-      <c r="E58" s="37">
+      <c r="E58" s="34">
         <v>1.4</v>
       </c>
       <c r="F58" s="8">
@@ -4968,15 +4968,15 @@
       <c r="X58" s="9"/>
       <c r="Y58" s="9"/>
       <c r="Z58" s="12"/>
-      <c r="AA58" s="32"/>
-      <c r="AB58" s="32"/>
+      <c r="AA58" s="36"/>
+      <c r="AB58" s="36"/>
       <c r="AC58" s="8"/>
       <c r="AD58" s="7"/>
       <c r="AE58" s="11"/>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A59" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B59" s="26">
         <v>87</v>
@@ -4987,7 +4987,7 @@
       <c r="D59" s="7">
         <v>0.69</v>
       </c>
-      <c r="E59" s="37">
+      <c r="E59" s="34">
         <v>1.6</v>
       </c>
       <c r="F59" s="8">
@@ -5025,15 +5025,15 @@
       <c r="X59" s="9"/>
       <c r="Y59" s="9"/>
       <c r="Z59" s="12"/>
-      <c r="AA59" s="32"/>
-      <c r="AB59" s="32"/>
+      <c r="AA59" s="36"/>
+      <c r="AB59" s="36"/>
       <c r="AC59" s="8"/>
       <c r="AD59" s="7"/>
       <c r="AE59" s="11"/>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A60" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B60" s="26">
         <v>87</v>
@@ -5044,7 +5044,7 @@
       <c r="D60" s="7">
         <v>0.69</v>
       </c>
-      <c r="E60" s="37">
+      <c r="E60" s="34">
         <v>1.8</v>
       </c>
       <c r="F60" s="8">
@@ -5078,15 +5078,15 @@
       <c r="X60" s="9"/>
       <c r="Y60" s="9"/>
       <c r="Z60" s="12"/>
-      <c r="AA60" s="32"/>
-      <c r="AB60" s="32"/>
+      <c r="AA60" s="36"/>
+      <c r="AB60" s="36"/>
       <c r="AC60" s="8"/>
       <c r="AD60" s="7"/>
       <c r="AE60" s="11"/>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B61" s="26">
         <v>87</v>
@@ -5097,7 +5097,7 @@
       <c r="D61" s="7">
         <v>0.69</v>
       </c>
-      <c r="E61" s="37">
+      <c r="E61" s="34">
         <v>2.1</v>
       </c>
       <c r="F61" s="8">
@@ -5135,15 +5135,15 @@
       <c r="X61" s="9"/>
       <c r="Y61" s="9"/>
       <c r="Z61" s="12"/>
-      <c r="AA61" s="32"/>
-      <c r="AB61" s="32"/>
+      <c r="AA61" s="36"/>
+      <c r="AB61" s="36"/>
       <c r="AC61" s="8"/>
       <c r="AD61" s="7"/>
       <c r="AE61" s="11"/>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A62" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B62" s="26">
         <v>87</v>
@@ -5154,7 +5154,7 @@
       <c r="D62" s="7">
         <v>0.69</v>
       </c>
-      <c r="E62" s="37">
+      <c r="E62" s="34">
         <v>2.2999999999999998</v>
       </c>
       <c r="F62" s="8">
@@ -5216,8 +5216,8 @@
         <v>3.82</v>
       </c>
       <c r="Z62" s="12"/>
-      <c r="AA62" s="32"/>
-      <c r="AB62" s="32"/>
+      <c r="AA62" s="36"/>
+      <c r="AB62" s="36"/>
       <c r="AC62" s="8"/>
       <c r="AD62" s="7">
         <v>3.2</v>
@@ -5228,7 +5228,7 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A63" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B63" s="26">
         <v>87</v>
@@ -5239,7 +5239,7 @@
       <c r="D63" s="7">
         <v>0.69</v>
       </c>
-      <c r="E63" s="37">
+      <c r="E63" s="34">
         <v>2.6</v>
       </c>
       <c r="F63" s="8">
@@ -5301,8 +5301,8 @@
         <v>2.73</v>
       </c>
       <c r="Z63" s="12"/>
-      <c r="AA63" s="32"/>
-      <c r="AB63" s="32"/>
+      <c r="AA63" s="36"/>
+      <c r="AB63" s="36"/>
       <c r="AC63" s="8"/>
       <c r="AD63" s="7">
         <v>3.01</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A64" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B64" s="26">
         <v>87</v>
@@ -5324,7 +5324,7 @@
       <c r="D64" s="7">
         <v>0.69</v>
       </c>
-      <c r="E64" s="37">
+      <c r="E64" s="34">
         <v>2.8</v>
       </c>
       <c r="F64" s="8">
@@ -5390,10 +5390,10 @@
       <c r="Z64" s="10">
         <v>8.6300000000000008</v>
       </c>
-      <c r="AA64" s="32">
+      <c r="AA64" s="36">
         <v>0.08</v>
       </c>
-      <c r="AB64" s="32"/>
+      <c r="AB64" s="36"/>
       <c r="AC64" s="8">
         <v>3.15</v>
       </c>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A65" s="30">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B65" s="26">
         <v>87</v>
@@ -5417,7 +5417,7 @@
       <c r="D65" s="7">
         <v>0.69</v>
       </c>
-      <c r="E65" s="37">
+      <c r="E65" s="34">
         <v>3</v>
       </c>
       <c r="F65" s="8">
@@ -5479,10 +5479,10 @@
       <c r="Z65" s="10">
         <v>16.68</v>
       </c>
-      <c r="AA65" s="32">
+      <c r="AA65" s="36">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AB65" s="32"/>
+      <c r="AB65" s="36"/>
       <c r="AC65" s="8">
         <v>2.96</v>
       </c>
@@ -5495,7 +5495,7 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B66" s="26">
         <v>96</v>
@@ -5506,7 +5506,7 @@
       <c r="D66" s="7">
         <v>0.6</v>
       </c>
-      <c r="E66" s="37">
+      <c r="E66" s="34">
         <v>0.8</v>
       </c>
       <c r="F66" s="8">
@@ -5570,8 +5570,8 @@
         <v>3.93</v>
       </c>
       <c r="Z66" s="12"/>
-      <c r="AA66" s="32"/>
-      <c r="AB66" s="32"/>
+      <c r="AA66" s="36"/>
+      <c r="AB66" s="36"/>
       <c r="AC66" s="8"/>
       <c r="AD66" s="7">
         <v>1.79</v>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A67" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B67" s="26">
         <v>96</v>
@@ -5593,7 +5593,7 @@
       <c r="D67" s="7">
         <v>0.6</v>
       </c>
-      <c r="E67" s="37">
+      <c r="E67" s="34">
         <v>1</v>
       </c>
       <c r="F67" s="8">
@@ -5631,15 +5631,15 @@
       <c r="X67" s="9"/>
       <c r="Y67" s="9"/>
       <c r="Z67" s="12"/>
-      <c r="AA67" s="32"/>
-      <c r="AB67" s="32"/>
+      <c r="AA67" s="36"/>
+      <c r="AB67" s="36"/>
       <c r="AC67" s="8"/>
       <c r="AD67" s="7"/>
       <c r="AE67" s="11"/>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A68" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B68" s="26">
         <v>96</v>
@@ -5650,7 +5650,7 @@
       <c r="D68" s="7">
         <v>0.6</v>
       </c>
-      <c r="E68" s="37">
+      <c r="E68" s="34">
         <v>1.3</v>
       </c>
       <c r="F68" s="8">
@@ -5688,15 +5688,15 @@
       <c r="X68" s="9"/>
       <c r="Y68" s="9"/>
       <c r="Z68" s="12"/>
-      <c r="AA68" s="32"/>
-      <c r="AB68" s="32"/>
+      <c r="AA68" s="36"/>
+      <c r="AB68" s="36"/>
       <c r="AC68" s="8"/>
       <c r="AD68" s="7"/>
       <c r="AE68" s="11"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A69" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B69" s="26">
         <v>96</v>
@@ -5707,7 +5707,7 @@
       <c r="D69" s="7">
         <v>0.6</v>
       </c>
-      <c r="E69" s="37">
+      <c r="E69" s="34">
         <v>1.6</v>
       </c>
       <c r="F69" s="8">
@@ -5741,15 +5741,15 @@
       <c r="X69" s="9"/>
       <c r="Y69" s="9"/>
       <c r="Z69" s="12"/>
-      <c r="AA69" s="32"/>
-      <c r="AB69" s="32"/>
+      <c r="AA69" s="36"/>
+      <c r="AB69" s="36"/>
       <c r="AC69" s="8"/>
       <c r="AD69" s="7"/>
       <c r="AE69" s="11"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A70" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B70" s="26">
         <v>96</v>
@@ -5760,7 +5760,7 @@
       <c r="D70" s="7">
         <v>0.6</v>
       </c>
-      <c r="E70" s="37">
+      <c r="E70" s="34">
         <v>1.8</v>
       </c>
       <c r="F70" s="8">
@@ -5794,15 +5794,15 @@
       <c r="X70" s="9"/>
       <c r="Y70" s="9"/>
       <c r="Z70" s="12"/>
-      <c r="AA70" s="32"/>
-      <c r="AB70" s="32"/>
+      <c r="AA70" s="36"/>
+      <c r="AB70" s="36"/>
       <c r="AC70" s="8"/>
       <c r="AD70" s="7"/>
       <c r="AE70" s="11"/>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A71" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B71" s="26">
         <v>96</v>
@@ -5813,7 +5813,7 @@
       <c r="D71" s="7">
         <v>0.6</v>
       </c>
-      <c r="E71" s="37">
+      <c r="E71" s="34">
         <v>2.1</v>
       </c>
       <c r="F71" s="8">
@@ -5851,15 +5851,15 @@
       <c r="X71" s="9"/>
       <c r="Y71" s="9"/>
       <c r="Z71" s="12"/>
-      <c r="AA71" s="32"/>
-      <c r="AB71" s="32"/>
+      <c r="AA71" s="36"/>
+      <c r="AB71" s="36"/>
       <c r="AC71" s="8"/>
       <c r="AD71" s="7"/>
       <c r="AE71" s="11"/>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A72" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B72" s="26">
         <v>96</v>
@@ -5870,7 +5870,7 @@
       <c r="D72" s="7">
         <v>0.6</v>
       </c>
-      <c r="E72" s="37">
+      <c r="E72" s="34">
         <v>2.2999999999999998</v>
       </c>
       <c r="F72" s="8">
@@ -5904,15 +5904,15 @@
       <c r="X72" s="9"/>
       <c r="Y72" s="9"/>
       <c r="Z72" s="12"/>
-      <c r="AA72" s="32"/>
-      <c r="AB72" s="32"/>
+      <c r="AA72" s="36"/>
+      <c r="AB72" s="36"/>
       <c r="AC72" s="8"/>
       <c r="AD72" s="7"/>
       <c r="AE72" s="11"/>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A73" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B73" s="26">
         <v>96</v>
@@ -5923,7 +5923,7 @@
       <c r="D73" s="7">
         <v>0.6</v>
       </c>
-      <c r="E73" s="37">
+      <c r="E73" s="34">
         <v>2.5</v>
       </c>
       <c r="F73" s="8">
@@ -5987,15 +5987,15 @@
         <v>4.12</v>
       </c>
       <c r="Z73" s="12"/>
-      <c r="AA73" s="32"/>
-      <c r="AB73" s="32"/>
+      <c r="AA73" s="36"/>
+      <c r="AB73" s="36"/>
       <c r="AC73" s="8"/>
       <c r="AD73" s="7"/>
       <c r="AE73" s="11"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A74" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B74" s="26">
         <v>96</v>
@@ -6006,7 +6006,7 @@
       <c r="D74" s="7">
         <v>0.6</v>
       </c>
-      <c r="E74" s="37">
+      <c r="E74" s="34">
         <v>2.8</v>
       </c>
       <c r="F74" s="8">
@@ -6070,8 +6070,8 @@
         <v>4.87</v>
       </c>
       <c r="Z74" s="12"/>
-      <c r="AA74" s="32"/>
-      <c r="AB74" s="32"/>
+      <c r="AA74" s="36"/>
+      <c r="AB74" s="36"/>
       <c r="AC74" s="8"/>
       <c r="AD74" s="7">
         <v>1.84</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A75" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B75" s="26">
         <v>96</v>
@@ -6093,7 +6093,7 @@
       <c r="D75" s="7">
         <v>0.6</v>
       </c>
-      <c r="E75" s="37">
+      <c r="E75" s="34">
         <v>3</v>
       </c>
       <c r="F75" s="8">
@@ -6157,8 +6157,8 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="Z75" s="12"/>
-      <c r="AA75" s="32"/>
-      <c r="AB75" s="32"/>
+      <c r="AA75" s="36"/>
+      <c r="AB75" s="36"/>
       <c r="AC75" s="8"/>
       <c r="AD75" s="7">
         <v>1.87</v>
@@ -6169,7 +6169,7 @@
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A76" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B76" s="26">
         <v>96</v>
@@ -6180,7 +6180,7 @@
       <c r="D76" s="7">
         <v>0.6</v>
       </c>
-      <c r="E76" s="37">
+      <c r="E76" s="34">
         <v>3.2</v>
       </c>
       <c r="F76" s="8">
@@ -6240,8 +6240,8 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="Z76" s="12"/>
-      <c r="AA76" s="32"/>
-      <c r="AB76" s="32"/>
+      <c r="AA76" s="36"/>
+      <c r="AB76" s="36"/>
       <c r="AC76" s="8"/>
       <c r="AD76" s="7">
         <v>1.91</v>
@@ -6252,7 +6252,7 @@
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A77" s="31">
-        <v>43187</v>
+        <v>42091</v>
       </c>
       <c r="B77" s="27">
         <v>87</v>
@@ -6260,7 +6260,7 @@
       <c r="C77" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E77" s="37">
+      <c r="E77" s="34">
         <v>0</v>
       </c>
       <c r="F77" s="8">
@@ -6310,8 +6310,8 @@
         <v>4.76</v>
       </c>
       <c r="Z77" s="12"/>
-      <c r="AA77" s="32"/>
-      <c r="AB77" s="32"/>
+      <c r="AA77" s="36"/>
+      <c r="AB77" s="36"/>
       <c r="AC77" s="8"/>
       <c r="AD77" s="7">
         <v>2.41</v>
@@ -6322,7 +6322,7 @@
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A78" s="31">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B78" s="27">
         <v>96</v>
@@ -6330,7 +6330,7 @@
       <c r="C78" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E78" s="37">
+      <c r="E78" s="34">
         <v>0</v>
       </c>
       <c r="F78" s="8">
@@ -6382,8 +6382,8 @@
       <c r="Z78" s="10">
         <v>0.26</v>
       </c>
-      <c r="AA78" s="32"/>
-      <c r="AB78" s="32"/>
+      <c r="AA78" s="36"/>
+      <c r="AB78" s="36"/>
       <c r="AC78" s="8"/>
       <c r="AD78" s="7">
         <v>1.64</v>
@@ -6394,6 +6394,70 @@
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AA27:AB27"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="AA24:AB24"/>
+    <mergeCell ref="AA25:AB25"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AA28:AB28"/>
+    <mergeCell ref="AA29:AB29"/>
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AA32:AB32"/>
+    <mergeCell ref="AA43:AB43"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="AA35:AB35"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="AA38:AB38"/>
+    <mergeCell ref="AA39:AB39"/>
+    <mergeCell ref="AA40:AB40"/>
+    <mergeCell ref="AA41:AB41"/>
+    <mergeCell ref="AA42:AB42"/>
+    <mergeCell ref="AA37:AB37"/>
+    <mergeCell ref="AA54:AB54"/>
+    <mergeCell ref="AA44:AB44"/>
+    <mergeCell ref="AA45:AB45"/>
+    <mergeCell ref="AA46:AB46"/>
+    <mergeCell ref="AA47:AB47"/>
+    <mergeCell ref="AA48:AB48"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="AA50:AB50"/>
+    <mergeCell ref="AA51:AB51"/>
+    <mergeCell ref="AA52:AB52"/>
+    <mergeCell ref="AA53:AB53"/>
+    <mergeCell ref="AA65:AB65"/>
+    <mergeCell ref="AA55:AB55"/>
+    <mergeCell ref="AA56:AB56"/>
+    <mergeCell ref="AA57:AB57"/>
+    <mergeCell ref="AA58:AB58"/>
+    <mergeCell ref="AA59:AB59"/>
+    <mergeCell ref="AA60:AB60"/>
+    <mergeCell ref="AA61:AB61"/>
+    <mergeCell ref="AA62:AB62"/>
+    <mergeCell ref="AA63:AB63"/>
+    <mergeCell ref="AA64:AB64"/>
     <mergeCell ref="AA77:AB77"/>
     <mergeCell ref="AA78:AB78"/>
     <mergeCell ref="AA76:AB76"/>
@@ -6407,70 +6471,6 @@
     <mergeCell ref="AA73:AB73"/>
     <mergeCell ref="AA74:AB74"/>
     <mergeCell ref="AA75:AB75"/>
-    <mergeCell ref="AA65:AB65"/>
-    <mergeCell ref="AA55:AB55"/>
-    <mergeCell ref="AA56:AB56"/>
-    <mergeCell ref="AA57:AB57"/>
-    <mergeCell ref="AA58:AB58"/>
-    <mergeCell ref="AA59:AB59"/>
-    <mergeCell ref="AA60:AB60"/>
-    <mergeCell ref="AA61:AB61"/>
-    <mergeCell ref="AA62:AB62"/>
-    <mergeCell ref="AA63:AB63"/>
-    <mergeCell ref="AA64:AB64"/>
-    <mergeCell ref="AA54:AB54"/>
-    <mergeCell ref="AA44:AB44"/>
-    <mergeCell ref="AA45:AB45"/>
-    <mergeCell ref="AA46:AB46"/>
-    <mergeCell ref="AA47:AB47"/>
-    <mergeCell ref="AA48:AB48"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="AA50:AB50"/>
-    <mergeCell ref="AA51:AB51"/>
-    <mergeCell ref="AA52:AB52"/>
-    <mergeCell ref="AA53:AB53"/>
-    <mergeCell ref="AA43:AB43"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AA35:AB35"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="AA38:AB38"/>
-    <mergeCell ref="AA39:AB39"/>
-    <mergeCell ref="AA40:AB40"/>
-    <mergeCell ref="AA41:AB41"/>
-    <mergeCell ref="AA42:AB42"/>
-    <mergeCell ref="AA37:AB37"/>
-    <mergeCell ref="AA28:AB28"/>
-    <mergeCell ref="AA29:AB29"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AA32:AB32"/>
-    <mergeCell ref="AA27:AB27"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AA25:AB25"/>
-    <mergeCell ref="AA26:AB26"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AA9:AB9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6569,10 +6569,10 @@
       <c r="AA1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AB1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="33"/>
+      <c r="AC1" s="37"/>
       <c r="AD1" s="2" t="s">
         <v>37</v>
       </c>
@@ -6641,7 +6641,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B3" s="26">
         <v>15</v>
@@ -6721,7 +6721,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B4" s="26">
         <v>15</v>
@@ -6777,7 +6777,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B5" s="26">
         <v>15</v>
@@ -6827,7 +6827,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B6" s="26">
         <v>15</v>
@@ -6883,7 +6883,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B7" s="26">
         <v>15</v>
@@ -6933,7 +6933,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B8" s="26">
         <v>15</v>
@@ -6989,7 +6989,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B9" s="26">
         <v>15</v>
@@ -7043,7 +7043,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B10" s="26">
         <v>15</v>
@@ -7095,7 +7095,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B11" s="26">
         <v>15</v>
@@ -7149,7 +7149,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B12" s="26">
         <v>15</v>
@@ -7201,7 +7201,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B13" s="26">
         <v>15</v>
@@ -7273,7 +7273,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B14" s="26">
         <v>15</v>
@@ -7325,7 +7325,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B15" s="26">
         <v>15</v>
@@ -7405,7 +7405,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B16" s="26">
         <v>15</v>
@@ -7479,7 +7479,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
-        <v>43115</v>
+        <v>42019</v>
       </c>
       <c r="B17" s="26">
         <v>15</v>
@@ -7559,7 +7559,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B18" s="26">
         <v>37</v>
@@ -7651,7 +7651,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B19" s="26">
         <v>37</v>
@@ -7707,7 +7707,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B20" s="26">
         <v>37</v>
@@ -7763,7 +7763,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B21" s="26">
         <v>37</v>
@@ -7819,7 +7819,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B22" s="26">
         <v>37</v>
@@ -7871,7 +7871,7 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B23" s="26">
         <v>37</v>
@@ -7927,7 +7927,7 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B24" s="26">
         <v>37</v>
@@ -7983,7 +7983,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B25" s="26">
         <v>37</v>
@@ -8039,7 +8039,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B26" s="26">
         <v>37</v>
@@ -8121,7 +8121,7 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B27" s="26">
         <v>37</v>
@@ -8213,7 +8213,7 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B28" s="26">
         <v>37</v>
@@ -8299,7 +8299,7 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
-        <v>43137</v>
+        <v>42041</v>
       </c>
       <c r="B29" s="26">
         <v>37</v>
@@ -8391,7 +8391,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B30" s="26">
         <v>49</v>
@@ -8483,7 +8483,7 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B31" s="26">
         <v>49</v>
@@ -8539,7 +8539,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B32" s="26">
         <v>49</v>
@@ -8595,7 +8595,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B33" s="26">
         <v>49</v>
@@ -8647,7 +8647,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B34" s="26">
         <v>49</v>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B35" s="26">
         <v>49</v>
@@ -8787,7 +8787,7 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B36" s="26">
         <v>49</v>
@@ -8843,7 +8843,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B37" s="26">
         <v>49</v>
@@ -8929,7 +8929,7 @@
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B38" s="26">
         <v>49</v>
@@ -9021,7 +9021,7 @@
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="30">
-        <v>43149</v>
+        <v>42053</v>
       </c>
       <c r="B39" s="26">
         <v>49</v>
@@ -9113,7 +9113,7 @@
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B40" s="26">
         <v>69</v>
@@ -9205,7 +9205,7 @@
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B41" s="26">
         <v>69</v>
@@ -9261,7 +9261,7 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B42" s="26">
         <v>69</v>
@@ -9313,7 +9313,7 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B43" s="26">
         <v>69</v>
@@ -9369,7 +9369,7 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B44" s="26">
         <v>69</v>
@@ -9421,7 +9421,7 @@
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B45" s="26">
         <v>69</v>
@@ -9477,7 +9477,7 @@
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B46" s="26">
         <v>69</v>
@@ -9529,7 +9529,7 @@
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B47" s="26">
         <v>69</v>
@@ -9585,7 +9585,7 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B48" s="26">
         <v>69</v>
@@ -9637,7 +9637,7 @@
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B49" s="26">
         <v>69</v>
@@ -9693,7 +9693,7 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B50" s="26">
         <v>69</v>
@@ -9745,7 +9745,7 @@
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B51" s="26">
         <v>69</v>
@@ -9801,7 +9801,7 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B52" s="26">
         <v>69</v>
@@ -9883,7 +9883,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B53" s="26">
         <v>69</v>
@@ -9969,7 +9969,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B54" s="26">
         <v>69</v>
@@ -10061,7 +10061,7 @@
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="30">
-        <v>43169</v>
+        <v>42073</v>
       </c>
       <c r="B55" s="26">
         <v>69</v>
@@ -10153,7 +10153,7 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B56" s="26">
         <v>78</v>
@@ -10245,7 +10245,7 @@
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B57" s="26">
         <v>78</v>
@@ -10301,7 +10301,7 @@
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B58" s="26">
         <v>78</v>
@@ -10353,7 +10353,7 @@
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B59" s="26">
         <v>78</v>
@@ -10409,7 +10409,7 @@
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B60" s="26">
         <v>78</v>
@@ -10461,7 +10461,7 @@
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B61" s="26">
         <v>78</v>
@@ -10517,7 +10517,7 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B62" s="26">
         <v>78</v>
@@ -10569,7 +10569,7 @@
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B63" s="26">
         <v>78</v>
@@ -10625,7 +10625,7 @@
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B64" s="26">
         <v>78</v>
@@ -10677,7 +10677,7 @@
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B65" s="26">
         <v>78</v>
@@ -10733,7 +10733,7 @@
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B66" s="26">
         <v>78</v>
@@ -10785,7 +10785,7 @@
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B67" s="26">
         <v>78</v>
@@ -10871,7 +10871,7 @@
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B68" s="26">
         <v>78</v>
@@ -10923,7 +10923,7 @@
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B69" s="26">
         <v>78</v>
@@ -11009,7 +11009,7 @@
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B70" s="26">
         <v>78</v>
@@ -11101,7 +11101,7 @@
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" s="30">
-        <v>43178</v>
+        <v>42082</v>
       </c>
       <c r="B71" s="26">
         <v>78</v>
@@ -11193,7 +11193,7 @@
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B72" s="26">
         <v>84</v>
@@ -11285,7 +11285,7 @@
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B73" s="26">
         <v>84</v>
@@ -11341,7 +11341,7 @@
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B74" s="26">
         <v>84</v>
@@ -11397,7 +11397,7 @@
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B75" s="26">
         <v>84</v>
@@ -11453,7 +11453,7 @@
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B76" s="26">
         <v>84</v>
@@ -11509,7 +11509,7 @@
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B77" s="26">
         <v>84</v>
@@ -11565,7 +11565,7 @@
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B78" s="26">
         <v>84</v>
@@ -11621,7 +11621,7 @@
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B79" s="26">
         <v>84</v>
@@ -11677,7 +11677,7 @@
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B80" s="26">
         <v>84</v>
@@ -11733,7 +11733,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B81" s="26">
         <v>84</v>
@@ -11789,7 +11789,7 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B82" s="26">
         <v>84</v>
@@ -11845,7 +11845,7 @@
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B83" s="26">
         <v>84</v>
@@ -11901,7 +11901,7 @@
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B84" s="26">
         <v>84</v>
@@ -11987,7 +11987,7 @@
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B85" s="26">
         <v>84</v>
@@ -12043,7 +12043,7 @@
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B86" s="26">
         <v>84</v>
@@ -12129,7 +12129,7 @@
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B87" s="26">
         <v>84</v>
@@ -12221,7 +12221,7 @@
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="30">
-        <v>43184</v>
+        <v>42088</v>
       </c>
       <c r="B88" s="26">
         <v>84</v>
@@ -12309,7 +12309,7 @@
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B89" s="26">
         <v>86</v>
@@ -12401,7 +12401,7 @@
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B90" s="26">
         <v>86</v>
@@ -12453,7 +12453,7 @@
     </row>
     <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B91" s="26">
         <v>86</v>
@@ -12509,7 +12509,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B92" s="26">
         <v>86</v>
@@ -12561,7 +12561,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B93" s="26">
         <v>86</v>
@@ -12617,7 +12617,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B94" s="26">
         <v>86</v>
@@ -12669,7 +12669,7 @@
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B95" s="26">
         <v>86</v>
@@ -12725,7 +12725,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B96" s="26">
         <v>86</v>
@@ -12777,7 +12777,7 @@
     </row>
     <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B97" s="26">
         <v>86</v>
@@ -12833,7 +12833,7 @@
     </row>
     <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B98" s="26">
         <v>86</v>
@@ -12885,7 +12885,7 @@
     </row>
     <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B99" s="26">
         <v>86</v>
@@ -12937,7 +12937,7 @@
     </row>
     <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B100" s="26">
         <v>86</v>
@@ -12993,7 +12993,7 @@
     </row>
     <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B101" s="26">
         <v>86</v>
@@ -13049,7 +13049,7 @@
     </row>
     <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B102" s="26">
         <v>86</v>
@@ -13131,7 +13131,7 @@
     </row>
     <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B103" s="26">
         <v>86</v>
@@ -13183,7 +13183,7 @@
     </row>
     <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B104" s="26">
         <v>86</v>
@@ -13269,7 +13269,7 @@
     </row>
     <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B105" s="26">
         <v>86</v>
@@ -13355,7 +13355,7 @@
     </row>
     <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" s="30">
-        <v>43186</v>
+        <v>42090</v>
       </c>
       <c r="B106" s="26">
         <v>86</v>
@@ -13447,7 +13447,7 @@
     </row>
     <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B107" s="26">
         <v>96</v>
@@ -13539,7 +13539,7 @@
     </row>
     <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B108" s="26">
         <v>96</v>
@@ -13595,7 +13595,7 @@
     </row>
     <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B109" s="26">
         <v>96</v>
@@ -13647,7 +13647,7 @@
     </row>
     <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B110" s="26">
         <v>96</v>
@@ -13703,7 +13703,7 @@
     </row>
     <row r="111" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A111" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B111" s="26">
         <v>96</v>
@@ -13759,7 +13759,7 @@
     </row>
     <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B112" s="26">
         <v>96</v>
@@ -13811,7 +13811,7 @@
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A113" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B113" s="26">
         <v>96</v>
@@ -13867,7 +13867,7 @@
     </row>
     <row r="114" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A114" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B114" s="26">
         <v>96</v>
@@ -13919,7 +13919,7 @@
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B115" s="26">
         <v>96</v>
@@ -13971,7 +13971,7 @@
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A116" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B116" s="26">
         <v>96</v>
@@ -14027,7 +14027,7 @@
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B117" s="26">
         <v>96</v>
@@ -14079,7 +14079,7 @@
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A118" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B118" s="26">
         <v>96</v>
@@ -14135,7 +14135,7 @@
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B119" s="26">
         <v>96</v>
@@ -14187,7 +14187,7 @@
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B120" s="26">
         <v>96</v>
@@ -14243,7 +14243,7 @@
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B121" s="26">
         <v>96</v>
@@ -14325,7 +14325,7 @@
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A122" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B122" s="26">
         <v>96</v>
@@ -14381,7 +14381,7 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B123" s="26">
         <v>96</v>
@@ -14467,7 +14467,7 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A124" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B124" s="26">
         <v>96</v>
@@ -14553,7 +14553,7 @@
     </row>
     <row r="125" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="30">
-        <v>43196</v>
+        <v>42100</v>
       </c>
       <c r="B125" s="26">
         <v>96</v>

</xml_diff>